<commit_message>
Laura created a graph for abundance vs. mean dbh
</commit_message>
<xml_diff>
--- a/sum_data.xlsx
+++ b/sum_data.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f2b00755eb3db8f8/Documents/Dissertation_proj/undergrad_dissertation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{09BDB0E3-6D41-484E-B986-6DCA03D1065A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="303" documentId="8_{09BDB0E3-6D41-484E-B986-6DCA03D1065A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7AD02EC4-9364-40ED-9DAD-5504D278D2A8}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6506EFFB-9B75-44E7-A6C3-92B03D2B76B8}"/>
+    <workbookView xWindow="0" yWindow="530" windowWidth="10040" windowHeight="9670" firstSheet="1" activeTab="2" xr2:uid="{6506EFFB-9B75-44E7-A6C3-92B03D2B76B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Count by family" sheetId="3" r:id="rId2"/>
+    <sheet name="INDICES" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="76">
   <si>
     <t>1A</t>
   </si>
@@ -196,6 +198,72 @@
   </si>
   <si>
     <t>other_d</t>
+  </si>
+  <si>
+    <t>Plot number</t>
+  </si>
+  <si>
+    <t>Number of saplings</t>
+  </si>
+  <si>
+    <t>Mean DBH of trees</t>
+  </si>
+  <si>
+    <t>Standard deviation of DBH measures</t>
+  </si>
+  <si>
+    <t>Number of stems/ plot</t>
+  </si>
+  <si>
+    <t>Last felled</t>
+  </si>
+  <si>
+    <t>No. of species</t>
+  </si>
+  <si>
+    <t>Total abundance</t>
+  </si>
+  <si>
+    <t>Menhinick's Richness Index</t>
+  </si>
+  <si>
+    <t>Margalef's Richness Index</t>
+  </si>
+  <si>
+    <t>Shannon-Weiner diversity Index</t>
+  </si>
+  <si>
+    <t>Simpson's Evenness Index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plot </t>
+  </si>
+  <si>
+    <t>Collembola</t>
+  </si>
+  <si>
+    <t>Dermaptera</t>
+  </si>
+  <si>
+    <t>Hemiptera</t>
+  </si>
+  <si>
+    <t>Coleoptera</t>
+  </si>
+  <si>
+    <t>Diptera</t>
+  </si>
+  <si>
+    <t>Hymenoptera</t>
+  </si>
+  <si>
+    <t>Mollusca</t>
+  </si>
+  <si>
+    <t>Arachnida</t>
+  </si>
+  <si>
+    <t>Other</t>
   </si>
 </sst>
 </file>
@@ -219,12 +287,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -239,9 +313,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -558,8 +634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D33DB738-04C4-44B8-B74A-A254C1AD364F}">
   <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:M43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -603,84 +679,84 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <v>4</v>
       </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
+      <c r="C2" s="3">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0</v>
+      </c>
+      <c r="G2" s="3">
         <v>4</v>
       </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
+      <c r="H2" s="3">
+        <v>0</v>
+      </c>
+      <c r="I2" s="3">
+        <v>0</v>
+      </c>
+      <c r="J2" s="3">
+        <v>1</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <v>0</v>
+      </c>
+      <c r="M2" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
+      <c r="B3" s="3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3">
         <v>3</v>
       </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>2</v>
-      </c>
-      <c r="H3">
+      <c r="E3" s="3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3">
+        <v>2</v>
+      </c>
+      <c r="H3" s="3">
         <v>3</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="3">
         <v>3</v>
       </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
+      <c r="J3" s="3">
+        <v>0</v>
+      </c>
+      <c r="K3" s="3">
+        <v>1</v>
+      </c>
+      <c r="L3" s="3">
+        <v>0</v>
+      </c>
+      <c r="M3" s="3">
         <v>0</v>
       </c>
     </row>
@@ -767,84 +843,84 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6">
+      <c r="B6" s="3">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3">
+        <v>0</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0</v>
+      </c>
+      <c r="K6" s="3">
+        <v>0</v>
+      </c>
+      <c r="L6" s="3">
+        <v>0</v>
+      </c>
+      <c r="M6" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
+      <c r="B7" s="3">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1</v>
+      </c>
+      <c r="E7" s="3">
         <v>9</v>
       </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7">
+      <c r="F7" s="3">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3">
         <v>3</v>
       </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>2</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7">
+      <c r="H7" s="3">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0</v>
+      </c>
+      <c r="J7" s="3">
+        <v>2</v>
+      </c>
+      <c r="K7" s="3">
+        <v>0</v>
+      </c>
+      <c r="L7" s="3">
+        <v>0</v>
+      </c>
+      <c r="M7" s="3">
         <v>0</v>
       </c>
     </row>
@@ -1013,535 +1089,535 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="3">
         <v>4</v>
       </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
+      <c r="C12" s="3">
+        <v>1</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1</v>
+      </c>
+      <c r="E12" s="3">
         <v>4</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="3">
         <v>4</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="3">
         <v>5</v>
       </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
-      <c r="J12">
-        <v>1</v>
-      </c>
-      <c r="K12">
+      <c r="H12" s="3">
+        <v>0</v>
+      </c>
+      <c r="I12" s="3">
+        <v>1</v>
+      </c>
+      <c r="J12" s="3">
+        <v>1</v>
+      </c>
+      <c r="K12" s="3">
         <v>4</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="3">
         <v>3</v>
       </c>
-      <c r="M12">
+      <c r="M12" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13">
+      <c r="B13" s="3">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3">
         <v>4</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="3">
         <v>3</v>
       </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>2</v>
-      </c>
-      <c r="J13">
-        <v>2</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
-      <c r="M13">
+      <c r="E13" s="3">
+        <v>1</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0</v>
+      </c>
+      <c r="G13" s="3">
+        <v>1</v>
+      </c>
+      <c r="H13" s="3">
+        <v>0</v>
+      </c>
+      <c r="I13" s="3">
+        <v>2</v>
+      </c>
+      <c r="J13" s="3">
+        <v>2</v>
+      </c>
+      <c r="K13" s="3">
+        <v>0</v>
+      </c>
+      <c r="L13" s="3">
+        <v>0</v>
+      </c>
+      <c r="M13" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B14">
-        <v>2</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14">
-        <v>1</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-      <c r="K14">
-        <v>0</v>
-      </c>
-      <c r="L14">
-        <v>0</v>
-      </c>
-      <c r="M14">
+      <c r="B14" s="3">
+        <v>2</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1</v>
+      </c>
+      <c r="D14" s="3">
+        <v>1</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0</v>
+      </c>
+      <c r="H14" s="3">
+        <v>1</v>
+      </c>
+      <c r="I14" s="3">
+        <v>0</v>
+      </c>
+      <c r="J14" s="3">
+        <v>0</v>
+      </c>
+      <c r="K14" s="3">
+        <v>0</v>
+      </c>
+      <c r="L14" s="3">
+        <v>0</v>
+      </c>
+      <c r="M14" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
-      <c r="M15">
+      <c r="B15" s="3">
+        <v>1</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0</v>
+      </c>
+      <c r="H15" s="3">
+        <v>0</v>
+      </c>
+      <c r="I15" s="3">
+        <v>0</v>
+      </c>
+      <c r="J15" s="3">
+        <v>0</v>
+      </c>
+      <c r="K15" s="3">
+        <v>0</v>
+      </c>
+      <c r="L15" s="3">
+        <v>0</v>
+      </c>
+      <c r="M15" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>2</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
-      <c r="L16">
-        <v>0</v>
-      </c>
-      <c r="M16">
+      <c r="B16" s="3">
+        <v>1</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0</v>
+      </c>
+      <c r="E16" s="3">
+        <v>2</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0</v>
+      </c>
+      <c r="G16" s="3">
+        <v>0</v>
+      </c>
+      <c r="H16" s="3">
+        <v>0</v>
+      </c>
+      <c r="I16" s="3">
+        <v>0</v>
+      </c>
+      <c r="J16" s="3">
+        <v>0</v>
+      </c>
+      <c r="K16" s="3">
+        <v>0</v>
+      </c>
+      <c r="L16" s="3">
+        <v>0</v>
+      </c>
+      <c r="M16" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
+      <c r="B17" s="3">
+        <v>0</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0</v>
+      </c>
+      <c r="D17" s="3">
         <v>4</v>
       </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
+      <c r="E17" s="3">
+        <v>0</v>
+      </c>
+      <c r="F17" s="3">
         <v>4</v>
       </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <v>1</v>
-      </c>
-      <c r="J17">
-        <v>0</v>
-      </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-      <c r="L17">
-        <v>1</v>
-      </c>
-      <c r="M17">
+      <c r="G17" s="3">
+        <v>0</v>
+      </c>
+      <c r="H17" s="3">
+        <v>0</v>
+      </c>
+      <c r="I17" s="3">
+        <v>1</v>
+      </c>
+      <c r="J17" s="3">
+        <v>0</v>
+      </c>
+      <c r="K17" s="3">
+        <v>0</v>
+      </c>
+      <c r="L17" s="3">
+        <v>1</v>
+      </c>
+      <c r="M17" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>2</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-      <c r="J18">
-        <v>0</v>
-      </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
-      <c r="M18">
+      <c r="B18" s="3">
+        <v>0</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0</v>
+      </c>
+      <c r="E18" s="3">
+        <v>2</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0</v>
+      </c>
+      <c r="G18" s="3">
+        <v>0</v>
+      </c>
+      <c r="H18" s="3">
+        <v>0</v>
+      </c>
+      <c r="I18" s="3">
+        <v>0</v>
+      </c>
+      <c r="J18" s="3">
+        <v>0</v>
+      </c>
+      <c r="K18" s="3">
+        <v>0</v>
+      </c>
+      <c r="L18" s="3">
+        <v>0</v>
+      </c>
+      <c r="M18" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
+      <c r="B19" s="3">
+        <v>0</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0</v>
+      </c>
+      <c r="F19" s="3">
         <v>7</v>
       </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <v>0</v>
-      </c>
-      <c r="J19">
-        <v>0</v>
-      </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-      <c r="L19">
-        <v>0</v>
-      </c>
-      <c r="M19">
+      <c r="G19" s="3">
+        <v>0</v>
+      </c>
+      <c r="H19" s="3">
+        <v>0</v>
+      </c>
+      <c r="I19" s="3">
+        <v>0</v>
+      </c>
+      <c r="J19" s="3">
+        <v>0</v>
+      </c>
+      <c r="K19" s="3">
+        <v>0</v>
+      </c>
+      <c r="L19" s="3">
+        <v>0</v>
+      </c>
+      <c r="M19" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B20">
-        <v>0</v>
-      </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <v>2</v>
-      </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-      <c r="J20">
-        <v>0</v>
-      </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-      <c r="L20">
-        <v>0</v>
-      </c>
-      <c r="M20">
+      <c r="B20" s="3">
+        <v>0</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0</v>
+      </c>
+      <c r="F20" s="3">
+        <v>2</v>
+      </c>
+      <c r="G20" s="3">
+        <v>0</v>
+      </c>
+      <c r="H20" s="3">
+        <v>0</v>
+      </c>
+      <c r="I20" s="3">
+        <v>0</v>
+      </c>
+      <c r="J20" s="3">
+        <v>0</v>
+      </c>
+      <c r="K20" s="3">
+        <v>0</v>
+      </c>
+      <c r="L20" s="3">
+        <v>0</v>
+      </c>
+      <c r="M20" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <v>1</v>
-      </c>
-      <c r="J21">
-        <v>0</v>
-      </c>
-      <c r="K21">
-        <v>0</v>
-      </c>
-      <c r="L21">
-        <v>0</v>
-      </c>
-      <c r="M21">
+      <c r="B21" s="3">
+        <v>0</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0</v>
+      </c>
+      <c r="F21" s="3">
+        <v>1</v>
+      </c>
+      <c r="G21" s="3">
+        <v>0</v>
+      </c>
+      <c r="H21" s="3">
+        <v>0</v>
+      </c>
+      <c r="I21" s="3">
+        <v>1</v>
+      </c>
+      <c r="J21" s="3">
+        <v>0</v>
+      </c>
+      <c r="K21" s="3">
+        <v>0</v>
+      </c>
+      <c r="L21" s="3">
+        <v>0</v>
+      </c>
+      <c r="M21" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B22">
-        <v>0</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22">
-        <v>1</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
-      <c r="J22">
-        <v>0</v>
-      </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-      <c r="L22">
-        <v>0</v>
-      </c>
-      <c r="M22">
+      <c r="B22" s="3">
+        <v>0</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0</v>
+      </c>
+      <c r="E22" s="3">
+        <v>0</v>
+      </c>
+      <c r="F22" s="3">
+        <v>1</v>
+      </c>
+      <c r="G22" s="3">
+        <v>0</v>
+      </c>
+      <c r="H22" s="3">
+        <v>0</v>
+      </c>
+      <c r="I22" s="3">
+        <v>0</v>
+      </c>
+      <c r="J22" s="3">
+        <v>0</v>
+      </c>
+      <c r="K22" s="3">
+        <v>0</v>
+      </c>
+      <c r="L22" s="3">
+        <v>0</v>
+      </c>
+      <c r="M22" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B23">
-        <v>0</v>
-      </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23">
-        <v>0</v>
-      </c>
-      <c r="H23">
-        <v>0</v>
-      </c>
-      <c r="I23">
-        <v>0</v>
-      </c>
-      <c r="J23">
-        <v>0</v>
-      </c>
-      <c r="K23">
-        <v>2</v>
-      </c>
-      <c r="L23">
-        <v>0</v>
-      </c>
-      <c r="M23">
+      <c r="B23" s="3">
+        <v>0</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0</v>
+      </c>
+      <c r="F23" s="3">
+        <v>0</v>
+      </c>
+      <c r="G23" s="3">
+        <v>0</v>
+      </c>
+      <c r="H23" s="3">
+        <v>0</v>
+      </c>
+      <c r="I23" s="3">
+        <v>0</v>
+      </c>
+      <c r="J23" s="3">
+        <v>0</v>
+      </c>
+      <c r="K23" s="3">
+        <v>2</v>
+      </c>
+      <c r="L23" s="3">
+        <v>0</v>
+      </c>
+      <c r="M23" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B24">
-        <v>0</v>
-      </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-      <c r="G24">
-        <v>0</v>
-      </c>
-      <c r="H24">
-        <v>0</v>
-      </c>
-      <c r="I24">
-        <v>0</v>
-      </c>
-      <c r="J24">
-        <v>0</v>
-      </c>
-      <c r="K24">
-        <v>0</v>
-      </c>
-      <c r="L24">
-        <v>1</v>
-      </c>
-      <c r="M24">
+      <c r="B24" s="3">
+        <v>0</v>
+      </c>
+      <c r="C24" s="3">
+        <v>0</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0</v>
+      </c>
+      <c r="E24" s="3">
+        <v>0</v>
+      </c>
+      <c r="F24" s="3">
+        <v>0</v>
+      </c>
+      <c r="G24" s="3">
+        <v>0</v>
+      </c>
+      <c r="H24" s="3">
+        <v>0</v>
+      </c>
+      <c r="I24" s="3">
+        <v>0</v>
+      </c>
+      <c r="J24" s="3">
+        <v>0</v>
+      </c>
+      <c r="K24" s="3">
+        <v>0</v>
+      </c>
+      <c r="L24" s="3">
+        <v>1</v>
+      </c>
+      <c r="M24" s="3">
         <v>0</v>
       </c>
     </row>
@@ -1752,84 +1828,84 @@
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="3">
         <v>3</v>
       </c>
-      <c r="C30">
-        <v>0</v>
-      </c>
-      <c r="D30">
-        <v>0</v>
-      </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
-      <c r="F30">
-        <v>0</v>
-      </c>
-      <c r="G30">
-        <v>0</v>
-      </c>
-      <c r="H30">
-        <v>0</v>
-      </c>
-      <c r="I30">
-        <v>0</v>
-      </c>
-      <c r="J30">
-        <v>0</v>
-      </c>
-      <c r="K30">
-        <v>2</v>
-      </c>
-      <c r="L30">
-        <v>0</v>
-      </c>
-      <c r="M30">
+      <c r="C30" s="3">
+        <v>0</v>
+      </c>
+      <c r="D30" s="3">
+        <v>0</v>
+      </c>
+      <c r="E30" s="3">
+        <v>0</v>
+      </c>
+      <c r="F30" s="3">
+        <v>0</v>
+      </c>
+      <c r="G30" s="3">
+        <v>0</v>
+      </c>
+      <c r="H30" s="3">
+        <v>0</v>
+      </c>
+      <c r="I30" s="3">
+        <v>0</v>
+      </c>
+      <c r="J30" s="3">
+        <v>0</v>
+      </c>
+      <c r="K30" s="3">
+        <v>2</v>
+      </c>
+      <c r="L30" s="3">
+        <v>0</v>
+      </c>
+      <c r="M30" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B31">
-        <v>0</v>
-      </c>
-      <c r="C31">
+      <c r="B31" s="3">
+        <v>0</v>
+      </c>
+      <c r="C31" s="3">
         <v>3</v>
       </c>
-      <c r="D31">
-        <v>0</v>
-      </c>
-      <c r="E31">
-        <v>1</v>
-      </c>
-      <c r="F31">
-        <v>0</v>
-      </c>
-      <c r="G31">
-        <v>0</v>
-      </c>
-      <c r="H31">
-        <v>0</v>
-      </c>
-      <c r="I31">
-        <v>0</v>
-      </c>
-      <c r="J31">
-        <v>0</v>
-      </c>
-      <c r="K31">
-        <v>0</v>
-      </c>
-      <c r="L31">
-        <v>0</v>
-      </c>
-      <c r="M31">
+      <c r="D31" s="3">
+        <v>0</v>
+      </c>
+      <c r="E31" s="3">
+        <v>1</v>
+      </c>
+      <c r="F31" s="3">
+        <v>0</v>
+      </c>
+      <c r="G31" s="3">
+        <v>0</v>
+      </c>
+      <c r="H31" s="3">
+        <v>0</v>
+      </c>
+      <c r="I31" s="3">
+        <v>0</v>
+      </c>
+      <c r="J31" s="3">
+        <v>0</v>
+      </c>
+      <c r="K31" s="3">
+        <v>0</v>
+      </c>
+      <c r="L31" s="3">
+        <v>0</v>
+      </c>
+      <c r="M31" s="3">
         <v>0</v>
       </c>
     </row>
@@ -2162,167 +2238,1204 @@
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A40" s="1" t="s">
+      <c r="A40" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B40">
-        <v>0</v>
-      </c>
-      <c r="C40">
-        <v>1</v>
-      </c>
-      <c r="D40">
-        <v>0</v>
-      </c>
-      <c r="E40">
-        <v>0</v>
-      </c>
-      <c r="F40">
-        <v>0</v>
-      </c>
-      <c r="G40">
-        <v>0</v>
-      </c>
-      <c r="H40">
-        <v>0</v>
-      </c>
-      <c r="I40">
-        <v>0</v>
-      </c>
-      <c r="J40">
-        <v>0</v>
-      </c>
-      <c r="K40">
-        <v>0</v>
-      </c>
-      <c r="L40">
-        <v>0</v>
-      </c>
-      <c r="M40">
+      <c r="B40" s="3">
+        <v>0</v>
+      </c>
+      <c r="C40" s="3">
+        <v>1</v>
+      </c>
+      <c r="D40" s="3">
+        <v>0</v>
+      </c>
+      <c r="E40" s="3">
+        <v>0</v>
+      </c>
+      <c r="F40" s="3">
+        <v>0</v>
+      </c>
+      <c r="G40" s="3">
+        <v>0</v>
+      </c>
+      <c r="H40" s="3">
+        <v>0</v>
+      </c>
+      <c r="I40" s="3">
+        <v>0</v>
+      </c>
+      <c r="J40" s="3">
+        <v>0</v>
+      </c>
+      <c r="K40" s="3">
+        <v>0</v>
+      </c>
+      <c r="L40" s="3">
+        <v>0</v>
+      </c>
+      <c r="M40" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A41" s="1" t="s">
+      <c r="A41" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B41">
-        <v>0</v>
-      </c>
-      <c r="C41">
-        <v>0</v>
-      </c>
-      <c r="D41">
-        <v>2</v>
-      </c>
-      <c r="E41">
-        <v>1</v>
-      </c>
-      <c r="F41">
-        <v>2</v>
-      </c>
-      <c r="G41">
-        <v>0</v>
-      </c>
-      <c r="H41">
-        <v>0</v>
-      </c>
-      <c r="I41">
-        <v>0</v>
-      </c>
-      <c r="J41">
-        <v>0</v>
-      </c>
-      <c r="K41">
-        <v>0</v>
-      </c>
-      <c r="L41">
-        <v>0</v>
-      </c>
-      <c r="M41">
+      <c r="B41" s="3">
+        <v>0</v>
+      </c>
+      <c r="C41" s="3">
+        <v>0</v>
+      </c>
+      <c r="D41" s="3">
+        <v>2</v>
+      </c>
+      <c r="E41" s="3">
+        <v>1</v>
+      </c>
+      <c r="F41" s="3">
+        <v>2</v>
+      </c>
+      <c r="G41" s="3">
+        <v>0</v>
+      </c>
+      <c r="H41" s="3">
+        <v>0</v>
+      </c>
+      <c r="I41" s="3">
+        <v>0</v>
+      </c>
+      <c r="J41" s="3">
+        <v>0</v>
+      </c>
+      <c r="K41" s="3">
+        <v>0</v>
+      </c>
+      <c r="L41" s="3">
+        <v>0</v>
+      </c>
+      <c r="M41" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A42" s="1" t="s">
+      <c r="A42" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B42">
-        <v>0</v>
-      </c>
-      <c r="C42">
-        <v>0</v>
-      </c>
-      <c r="D42">
-        <v>0</v>
-      </c>
-      <c r="E42">
-        <v>0</v>
-      </c>
-      <c r="F42">
+      <c r="B42" s="3">
+        <v>0</v>
+      </c>
+      <c r="C42" s="3">
+        <v>0</v>
+      </c>
+      <c r="D42" s="3">
+        <v>0</v>
+      </c>
+      <c r="E42" s="3">
+        <v>0</v>
+      </c>
+      <c r="F42" s="3">
         <v>18</v>
       </c>
-      <c r="G42">
-        <v>0</v>
-      </c>
-      <c r="H42">
-        <v>0</v>
-      </c>
-      <c r="I42">
-        <v>0</v>
-      </c>
-      <c r="J42">
-        <v>1</v>
-      </c>
-      <c r="K42">
-        <v>0</v>
-      </c>
-      <c r="L42">
-        <v>0</v>
-      </c>
-      <c r="M42">
+      <c r="G42" s="3">
+        <v>0</v>
+      </c>
+      <c r="H42" s="3">
+        <v>0</v>
+      </c>
+      <c r="I42" s="3">
+        <v>0</v>
+      </c>
+      <c r="J42" s="3">
+        <v>1</v>
+      </c>
+      <c r="K42" s="3">
+        <v>0</v>
+      </c>
+      <c r="L42" s="3">
+        <v>0</v>
+      </c>
+      <c r="M42" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A43" s="1" t="s">
+      <c r="A43" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B43">
-        <v>0</v>
-      </c>
-      <c r="C43">
-        <v>0</v>
-      </c>
-      <c r="D43">
-        <v>0</v>
-      </c>
-      <c r="E43">
-        <v>0</v>
-      </c>
-      <c r="F43">
-        <v>0</v>
-      </c>
-      <c r="G43">
-        <v>1</v>
-      </c>
-      <c r="H43">
-        <v>0</v>
-      </c>
-      <c r="I43">
-        <v>0</v>
-      </c>
-      <c r="J43">
-        <v>0</v>
-      </c>
-      <c r="K43">
-        <v>0</v>
-      </c>
-      <c r="L43">
-        <v>0</v>
-      </c>
-      <c r="M43">
-        <v>0</v>
+      <c r="B43" s="3">
+        <v>0</v>
+      </c>
+      <c r="C43" s="3">
+        <v>0</v>
+      </c>
+      <c r="D43" s="3">
+        <v>0</v>
+      </c>
+      <c r="E43" s="3">
+        <v>0</v>
+      </c>
+      <c r="F43" s="3">
+        <v>0</v>
+      </c>
+      <c r="G43" s="3">
+        <v>1</v>
+      </c>
+      <c r="H43" s="3">
+        <v>0</v>
+      </c>
+      <c r="I43" s="3">
+        <v>0</v>
+      </c>
+      <c r="J43" s="3">
+        <v>0</v>
+      </c>
+      <c r="K43" s="3">
+        <v>0</v>
+      </c>
+      <c r="L43" s="3">
+        <v>0</v>
+      </c>
+      <c r="M43" s="3">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C759B4B-258C-4985-A390-BC99224DE37E}">
+  <dimension ref="A1:J13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <f>SUM(Sheet1!B2:B3)</f>
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <f>SUM(Sheet1!B4:B5)</f>
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <f>SUM(Sheet1!B6:B7)</f>
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <f>SUM(Sheet1!B8:B11)</f>
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <f>SUM(Sheet1!B12:B24)</f>
+        <v>9</v>
+      </c>
+      <c r="G2">
+        <f>SUM(Sheet1!B25:B29)</f>
+        <v>29</v>
+      </c>
+      <c r="H2">
+        <f>SUM(Sheet1!B$30:B$31)</f>
+        <v>3</v>
+      </c>
+      <c r="I2">
+        <f>SUM(Sheet1!B$32:B$39)</f>
+        <v>5</v>
+      </c>
+      <c r="J2">
+        <f>SUM(Sheet1!B$40:B$43)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <f>SUM(Sheet1!C2:C3)</f>
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <f>SUM(Sheet1!C4:C5)</f>
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <f>SUM(Sheet1!C6:C7)</f>
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <f>SUM(Sheet1!C8:C11)</f>
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <f>SUM(Sheet1!C12:C24)</f>
+        <v>6</v>
+      </c>
+      <c r="G3">
+        <f>SUM(Sheet1!C$25:C$29)</f>
+        <v>30</v>
+      </c>
+      <c r="H3">
+        <f>SUM(Sheet1!C$30:C$31)</f>
+        <v>3</v>
+      </c>
+      <c r="I3">
+        <f>SUM(Sheet1!C$32:C$39)</f>
+        <v>6</v>
+      </c>
+      <c r="J3">
+        <f>SUM(Sheet1!C$40:C$43)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <f>SUM(Sheet1!D2:D3)</f>
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <f>SUM(Sheet1!D4:D5)</f>
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <f>SUM(Sheet1!D6:D7)</f>
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <f>SUM(Sheet1!D8:D11)</f>
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <f>SUM(Sheet1!D12:D24)</f>
+        <v>9</v>
+      </c>
+      <c r="G4">
+        <f>SUM(Sheet1!D$25:D$29)</f>
+        <v>11</v>
+      </c>
+      <c r="H4">
+        <f>SUM(Sheet1!D$30:D$31)</f>
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <f>SUM(Sheet1!D$32:D$39)</f>
+        <v>9</v>
+      </c>
+      <c r="J4">
+        <f>SUM(Sheet1!D$40:D$43)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <f>SUM(Sheet1!E2:E3)</f>
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <f>SUM(Sheet1!E$4:E$5)</f>
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <f>SUM(Sheet1!E6:E7)</f>
+        <v>9</v>
+      </c>
+      <c r="E5">
+        <f>SUM(Sheet1!E8:E11)</f>
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <f>SUM(Sheet1!E12:E24)</f>
+        <v>9</v>
+      </c>
+      <c r="G5">
+        <f>SUM(Sheet1!E$25:E$29)</f>
+        <v>6</v>
+      </c>
+      <c r="H5">
+        <f>SUM(Sheet1!E$30:E$31)</f>
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <f>SUM(Sheet1!E$32:E$39)</f>
+        <v>11</v>
+      </c>
+      <c r="J5">
+        <f>SUM(Sheet1!E$40:E$43)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <f>SUM(Sheet1!F2:F3)</f>
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <f>SUM(Sheet1!F4:F5)</f>
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <f>SUM(Sheet1!F6:F7)</f>
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <f>SUM(Sheet1!F8:F11)</f>
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <f>SUM(Sheet1!F12:F24)</f>
+        <v>19</v>
+      </c>
+      <c r="G6">
+        <f>SUM(Sheet1!F$25:F$29)</f>
+        <v>59</v>
+      </c>
+      <c r="H6">
+        <f>SUM(Sheet1!F$30:F$31)</f>
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <f>SUM(Sheet1!F$32:F$39)</f>
+        <v>6</v>
+      </c>
+      <c r="J6">
+        <f>SUM(Sheet1!F$40:F$43)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <f>SUM(Sheet1!G2:G3)</f>
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <f>SUM(Sheet1!G4:G5)</f>
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <f>SUM(Sheet1!G6:G7)</f>
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <f>SUM(Sheet1!G8:G11)</f>
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <f>SUM(Sheet1!G12:G24)</f>
+        <v>6</v>
+      </c>
+      <c r="G7">
+        <f>SUM(Sheet1!G$25:G$29)</f>
+        <v>112</v>
+      </c>
+      <c r="H7">
+        <f>SUM(Sheet1!G$30:G$31)</f>
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <f>SUM(Sheet1!G$32:G$39)</f>
+        <v>2</v>
+      </c>
+      <c r="J7">
+        <f>SUM(Sheet1!G$40:G$43)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <f>SUM(Sheet1!H2:H3)</f>
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <f>SUM(Sheet1!H4:H5)</f>
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <f>SUM(Sheet1!H6:H7)</f>
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <f>SUM(Sheet1!H8:H11)</f>
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <f>SUM(Sheet1!H12:H24)</f>
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <f>SUM(Sheet1!H$25:H$29)</f>
+        <v>4</v>
+      </c>
+      <c r="H8">
+        <f>SUM(Sheet1!H$30:H$31)</f>
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <f>SUM(Sheet1!H$32:H$39)</f>
+        <v>14</v>
+      </c>
+      <c r="J8">
+        <f>SUM(Sheet1!H$40:H$43)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <f>SUM(Sheet1!I2:I3)</f>
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <f>SUM(Sheet1!I4:I5)</f>
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <f>SUM(Sheet1!I6:I7)</f>
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <f>SUM(Sheet1!I8:I11)</f>
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <f>SUM(Sheet1!I12:I24)</f>
+        <v>5</v>
+      </c>
+      <c r="G9">
+        <f>SUM(Sheet1!I$25:I$29)</f>
+        <v>2</v>
+      </c>
+      <c r="H9">
+        <f>SUM(Sheet1!I$30:I$31)</f>
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <f>SUM(Sheet1!I$32:I$39)</f>
+        <v>7</v>
+      </c>
+      <c r="J9">
+        <f>SUM(Sheet1!I$40:I$43)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <f>SUM(Sheet1!J2:J3)</f>
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <f>SUM(Sheet1!J4:J5)</f>
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <f>SUM(Sheet1!J6:J7)</f>
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <f>SUM(Sheet1!J8:J11)</f>
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <f>SUM(Sheet1!J12:J24)</f>
+        <v>3</v>
+      </c>
+      <c r="G10">
+        <f>SUM(Sheet1!J$25:J$29)</f>
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <f>SUM(Sheet1!J$30:J$31)</f>
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <f>SUM(Sheet1!J$32:J$39)</f>
+        <v>2</v>
+      </c>
+      <c r="J10">
+        <f>SUM(Sheet1!J$40:J$43)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <f>SUM(Sheet1!K2:K3)</f>
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <f>SUM(Sheet1!K4:K5)</f>
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <f>SUM(Sheet1!K6:K7)</f>
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <f>SUM(Sheet1!K8:K11)</f>
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <f>SUM(Sheet1!K12:K24)</f>
+        <v>6</v>
+      </c>
+      <c r="G11">
+        <f>SUM(Sheet1!K$25:K$29)</f>
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <f>SUM(Sheet1!K$30:K$31)</f>
+        <v>2</v>
+      </c>
+      <c r="I11">
+        <f>SUM(Sheet1!K$32:K$39)</f>
+        <v>2</v>
+      </c>
+      <c r="J11">
+        <f>SUM(Sheet1!K$40:K$43)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <f>SUM(Sheet1!B12:B13)</f>
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <f>SUM(Sheet1!L4:L5)</f>
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <f>SUM(Sheet1!L6:L7)</f>
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <f>SUM(Sheet1!L8:L11)</f>
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <f>SUM(Sheet1!L12:L24)</f>
+        <v>5</v>
+      </c>
+      <c r="G12">
+        <f>SUM(Sheet1!L$25:L$29)</f>
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <f>SUM(Sheet1!L$30:L$31)</f>
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <f>SUM(Sheet1!L$32:L$39)</f>
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <f>SUM(Sheet1!L$40:L$43)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <f>SUM(Sheet1!M2:M3)</f>
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <f>SUM(Sheet1!M4:M5)</f>
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <f>SUM(Sheet1!M6:M7)</f>
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <f>SUM(Sheet1!M8:M11)</f>
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <f>SUM(Sheet1!M12:M24)</f>
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <f>SUM(Sheet1!M$25:M$29)</f>
+        <v>7</v>
+      </c>
+      <c r="H13">
+        <f>SUM(Sheet1!M$30:M$31)</f>
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <f>SUM(Sheet1!M$32:M$39)</f>
+        <v>2</v>
+      </c>
+      <c r="J13">
+        <f>SUM(Sheet1!M$40:M$43)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C30826F1-FD0F-4F5A-B821-6134EA477023}">
+  <dimension ref="A1:M12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:M7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="31.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2">
+        <v>1988</v>
+      </c>
+      <c r="C2">
+        <v>1988</v>
+      </c>
+      <c r="D2">
+        <v>1988</v>
+      </c>
+      <c r="E2">
+        <v>1988</v>
+      </c>
+      <c r="F2">
+        <v>1999</v>
+      </c>
+      <c r="G2">
+        <v>1999</v>
+      </c>
+      <c r="H2">
+        <v>1991</v>
+      </c>
+      <c r="I2">
+        <v>1991</v>
+      </c>
+      <c r="J2">
+        <v>2008</v>
+      </c>
+      <c r="K2">
+        <v>2008</v>
+      </c>
+      <c r="L2">
+        <v>2008</v>
+      </c>
+      <c r="M2">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3">
+        <v>16</v>
+      </c>
+      <c r="C3">
+        <v>15</v>
+      </c>
+      <c r="D3">
+        <v>16</v>
+      </c>
+      <c r="E3">
+        <v>14</v>
+      </c>
+      <c r="F3">
+        <v>17</v>
+      </c>
+      <c r="G3">
+        <v>12</v>
+      </c>
+      <c r="H3">
+        <v>10</v>
+      </c>
+      <c r="I3">
+        <v>9</v>
+      </c>
+      <c r="J3">
+        <v>7</v>
+      </c>
+      <c r="K3">
+        <v>6</v>
+      </c>
+      <c r="L3">
+        <v>3</v>
+      </c>
+      <c r="M3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4">
+        <v>52</v>
+      </c>
+      <c r="C4">
+        <v>53</v>
+      </c>
+      <c r="D4">
+        <v>38</v>
+      </c>
+      <c r="E4">
+        <v>39</v>
+      </c>
+      <c r="F4">
+        <v>107</v>
+      </c>
+      <c r="G4">
+        <v>132</v>
+      </c>
+      <c r="H4">
+        <v>24</v>
+      </c>
+      <c r="I4">
+        <v>17</v>
+      </c>
+      <c r="J4">
+        <v>10</v>
+      </c>
+      <c r="K4">
+        <v>12</v>
+      </c>
+      <c r="L4">
+        <v>10</v>
+      </c>
+      <c r="M4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5">
+        <f>(B3-1)/LN(B4)</f>
+        <v>3.796273039159753</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:M5" si="0">(C3-1)/LN(C4)</f>
+        <v>3.5261890825237954</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>4.1236136661374037</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>3.5484594653221664</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>3.4240500918845367</v>
+      </c>
+      <c r="G5">
+        <f>(G3-1)/LN(G4)</f>
+        <v>2.2528048801482843</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>2.8319218239971238</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>2.8236489909180893</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>2.6057668914195107</v>
+      </c>
+      <c r="K5">
+        <f>(K3-1)/LN(K4)</f>
+        <v>2.0121480219092232</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>0.86858896380650352</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="0"/>
+        <v>1.3028834457097553</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6">
+        <f>B3/SQRT(B4)</f>
+        <v>2.2188007849009166</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:M6" si="1">C3/SQRT(C4)</f>
+        <v>2.0604084592303353</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>2.5955427380922007</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>2.2417941532712198</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>1.643452031377628</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>1.044465935734187</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>2.0412414523193152</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>2.1828206253269968</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="1"/>
+        <v>2.2135943621178655</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="1"/>
+        <v>1.7320508075688774</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="1"/>
+        <v>0.94868329805051377</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="1"/>
+        <v>1.2649110640673518</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7">
+        <v>0.63979289940828399</v>
+      </c>
+      <c r="C7">
+        <v>0.62647015060619959</v>
+      </c>
+      <c r="D7">
+        <v>0.78947368421052633</v>
+      </c>
+      <c r="E7">
+        <v>0.78763971071663375</v>
+      </c>
+      <c r="F7">
+        <v>0.62590619268058356</v>
+      </c>
+      <c r="G7">
+        <v>0.27467860422405876</v>
+      </c>
+      <c r="H7">
+        <v>0.60763888888888884</v>
+      </c>
+      <c r="I7">
+        <v>0.69896193771626303</v>
+      </c>
+      <c r="J7">
+        <v>0.79999999999999993</v>
+      </c>
+      <c r="K7">
+        <v>0.68055555555555558</v>
+      </c>
+      <c r="L7">
+        <v>0.5</v>
+      </c>
+      <c r="M7">
+        <v>0.46000000000000008</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9">
+        <v>19</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>17</v>
+      </c>
+      <c r="E9">
+        <v>19</v>
+      </c>
+      <c r="F9">
+        <v>16</v>
+      </c>
+      <c r="G9">
+        <v>23</v>
+      </c>
+      <c r="H9">
+        <v>24</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>34</v>
+      </c>
+      <c r="K9">
+        <v>27</v>
+      </c>
+      <c r="L9">
+        <v>6</v>
+      </c>
+      <c r="M9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10">
+        <v>20.088235294117649</v>
+      </c>
+      <c r="C10">
+        <v>24.835000000000001</v>
+      </c>
+      <c r="D10">
+        <v>20.433333333333334</v>
+      </c>
+      <c r="E10">
+        <v>17.949999999999996</v>
+      </c>
+      <c r="F10">
+        <v>15.290909090909093</v>
+      </c>
+      <c r="G10">
+        <v>39.25</v>
+      </c>
+      <c r="H10">
+        <v>37.309090909090905</v>
+      </c>
+      <c r="I10">
+        <v>29.648387096774197</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11">
+        <v>10.822885610648225</v>
+      </c>
+      <c r="C11">
+        <v>14.49041924859319</v>
+      </c>
+      <c r="D11">
+        <v>18.212838878110134</v>
+      </c>
+      <c r="E11">
+        <v>5.0387446222666625</v>
+      </c>
+      <c r="F11">
+        <v>2.768918397300475</v>
+      </c>
+      <c r="G11">
+        <v>23.677588175702809</v>
+      </c>
+      <c r="H11">
+        <v>8.6028430818485351</v>
+      </c>
+      <c r="I11">
+        <v>6.8894543067764857</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12">
+        <v>36</v>
+      </c>
+      <c r="C12">
+        <v>18</v>
+      </c>
+      <c r="D12">
+        <v>26</v>
+      </c>
+      <c r="E12">
+        <v>39</v>
+      </c>
+      <c r="F12">
+        <v>27</v>
+      </c>
+      <c r="G12">
+        <v>35</v>
+      </c>
+      <c r="H12">
+        <v>35</v>
+      </c>
+      <c r="I12">
+        <v>31</v>
+      </c>
+      <c r="J12">
+        <v>34</v>
+      </c>
+      <c r="K12">
+        <v>27</v>
+      </c>
+      <c r="L12">
+        <v>6</v>
+      </c>
+      <c r="M12">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>